<commit_message>
Nowa wersja wizualizacji bramek logicznych
</commit_message>
<xml_diff>
--- a/Projekt.xlsx
+++ b/Projekt.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,16 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
   <si>
     <t>ArrayList&lt;type&gt;</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>NOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,8 +52,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,8 +92,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9191"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABE597"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -202,11 +250,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -239,6 +345,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -563,16 +688,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:AL28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.21875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.1796875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="2.21875" style="9"/>
+    <col min="1" max="16384" width="2.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U4" s="2"/>
       <c r="V4" s="11"/>
       <c r="W4" s="2"/>
@@ -580,7 +705,7 @@
       <c r="AB4" s="11"/>
       <c r="AC4" s="12"/>
     </row>
-    <row r="5" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S5" s="21"/>
       <c r="T5" s="22"/>
       <c r="U5" s="1"/>
@@ -592,7 +717,7 @@
       <c r="AB5" s="14"/>
       <c r="AC5" s="15"/>
     </row>
-    <row r="6" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S6" s="20"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
@@ -602,18 +727,18 @@
       <c r="AB6" s="17"/>
       <c r="AC6" s="18"/>
     </row>
-    <row r="9" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AL9" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
       <c r="G14" s="3"/>
       <c r="U14" s="31"/>
     </row>
-    <row r="15" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E15" s="26"/>
       <c r="F15" s="5"/>
       <c r="G15" s="27"/>
@@ -622,13 +747,13 @@
       <c r="W15" s="31"/>
       <c r="X15" s="31"/>
     </row>
-    <row r="16" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:38" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E16" s="4"/>
       <c r="F16" s="7"/>
       <c r="G16" s="6"/>
       <c r="X16" s="31"/>
     </row>
-    <row r="17" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T17" s="2"/>
       <c r="U17" s="8"/>
       <c r="V17" s="3"/>
@@ -636,7 +761,7 @@
       <c r="X17" s="28"/>
       <c r="Y17" s="3"/>
     </row>
-    <row r="18" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R18" s="31"/>
       <c r="S18" s="31"/>
       <c r="T18" s="30"/>
@@ -646,7 +771,7 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="27"/>
     </row>
-    <row r="19" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R19" s="31"/>
       <c r="T19" s="4"/>
       <c r="U19" s="7"/>
@@ -655,20 +780,20 @@
       <c r="X19" s="29"/>
       <c r="Y19" s="6"/>
     </row>
-    <row r="20" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R20" s="31"/>
       <c r="X20" s="31"/>
     </row>
-    <row r="21" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R21" s="31"/>
       <c r="X21" s="31"/>
       <c r="Y21" s="31"/>
     </row>
-    <row r="22" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R22" s="31"/>
       <c r="X22" s="31"/>
     </row>
-    <row r="23" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q23" s="2"/>
       <c r="R23" s="28"/>
       <c r="S23" s="3"/>
@@ -677,7 +802,7 @@
       <c r="V23" s="3"/>
       <c r="X23" s="31"/>
     </row>
-    <row r="24" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q24" s="26"/>
       <c r="R24" s="5"/>
       <c r="S24" s="19"/>
@@ -687,7 +812,7 @@
       <c r="W24" s="31"/>
       <c r="X24" s="31"/>
     </row>
-    <row r="25" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="Q25" s="4"/>
       <c r="R25" s="29"/>
       <c r="S25" s="6"/>
@@ -695,16 +820,16 @@
       <c r="U25" s="7"/>
       <c r="V25" s="6"/>
     </row>
-    <row r="26" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R26" s="31"/>
     </row>
-    <row r="27" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="R27" s="31"/>
       <c r="S27" s="31"/>
       <c r="T27" s="31"/>
       <c r="U27" s="31"/>
     </row>
-    <row r="28" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="17:25" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="U28" s="31"/>
     </row>
   </sheetData>
@@ -712,4 +837,717 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:DT69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P33" workbookViewId="0">
+      <selection activeCell="CR61" sqref="CR61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="1.6328125" defaultRowHeight="9" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CZ3" s="32"/>
+      <c r="DA3" s="33"/>
+    </row>
+    <row r="4" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CZ4" s="32"/>
+      <c r="DA4" s="33"/>
+    </row>
+    <row r="5" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CZ5" s="32"/>
+      <c r="DA5" s="33"/>
+    </row>
+    <row r="6" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CZ6" s="32"/>
+      <c r="DA6" s="33"/>
+    </row>
+    <row r="7" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
+      <c r="AE7" s="34"/>
+      <c r="AF7" s="34"/>
+      <c r="AG7" s="34"/>
+      <c r="AH7" s="34"/>
+      <c r="AI7" s="34"/>
+      <c r="AJ7" s="34"/>
+      <c r="CZ7" s="32"/>
+      <c r="DA7" s="33"/>
+    </row>
+    <row r="8" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CZ8" s="32"/>
+      <c r="DA8" s="33"/>
+    </row>
+    <row r="15" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="AD15" s="35"/>
+      <c r="AS15" s="35"/>
+      <c r="BH15" s="35"/>
+      <c r="BW15" s="35"/>
+    </row>
+    <row r="16" spans="5:120" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="AD16" s="35"/>
+      <c r="AS16" s="35"/>
+      <c r="BH16" s="35"/>
+      <c r="BW16" s="35"/>
+      <c r="CN16" s="35"/>
+      <c r="CV16" s="35"/>
+      <c r="DH16" s="36"/>
+      <c r="DP16" s="35"/>
+    </row>
+    <row r="17" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="AD17" s="35"/>
+      <c r="AS17" s="35"/>
+      <c r="BH17" s="35"/>
+      <c r="BW17" s="35"/>
+      <c r="CN17" s="35"/>
+      <c r="CV17" s="35"/>
+      <c r="DH17" s="36"/>
+      <c r="DP17" s="35"/>
+    </row>
+    <row r="18" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="AD18" s="35"/>
+      <c r="AS18" s="35"/>
+      <c r="BH18" s="35"/>
+      <c r="BW18" s="35"/>
+      <c r="CN18" s="35"/>
+      <c r="CV18" s="35"/>
+      <c r="DH18" s="36"/>
+      <c r="DP18" s="35"/>
+    </row>
+    <row r="19" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="AD19" s="35"/>
+      <c r="AS19" s="35"/>
+      <c r="BH19" s="35"/>
+      <c r="BW19" s="35"/>
+      <c r="CN19" s="35"/>
+      <c r="CV19" s="35"/>
+      <c r="DH19" s="36"/>
+      <c r="DP19" s="35"/>
+    </row>
+    <row r="20" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="AD20" s="35"/>
+      <c r="AS20" s="35"/>
+      <c r="BH20" s="35"/>
+      <c r="BW20" s="35"/>
+      <c r="CM20" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="CN20" s="38"/>
+      <c r="CO20" s="38"/>
+      <c r="CU20" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="CV20" s="38"/>
+      <c r="CW20" s="38"/>
+      <c r="DG20" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="DH20" s="38"/>
+      <c r="DI20" s="38"/>
+      <c r="DO20" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="DP20" s="38"/>
+      <c r="DQ20" s="38"/>
+    </row>
+    <row r="21" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AQ21" s="39"/>
+      <c r="AR21" s="35"/>
+      <c r="AS21" s="35"/>
+      <c r="AT21" s="35"/>
+      <c r="AU21" s="39"/>
+      <c r="BF21" s="39"/>
+      <c r="BG21" s="35"/>
+      <c r="BH21" s="35"/>
+      <c r="BI21" s="35"/>
+      <c r="BJ21" s="39"/>
+      <c r="BU21" s="39"/>
+      <c r="BV21" s="35"/>
+      <c r="BW21" s="35"/>
+      <c r="BX21" s="35"/>
+      <c r="BY21" s="39"/>
+      <c r="CM21" s="37"/>
+      <c r="CN21" s="38"/>
+      <c r="CO21" s="35"/>
+      <c r="CP21" s="35"/>
+      <c r="CQ21" s="35"/>
+      <c r="CR21" s="35"/>
+      <c r="CU21" s="37"/>
+      <c r="CV21" s="38"/>
+      <c r="CW21" s="40"/>
+      <c r="CX21" s="40"/>
+      <c r="CY21" s="40"/>
+      <c r="CZ21" s="40"/>
+      <c r="DG21" s="37"/>
+      <c r="DH21" s="38"/>
+      <c r="DI21" s="35"/>
+      <c r="DJ21" s="35"/>
+      <c r="DK21" s="35"/>
+      <c r="DL21" s="35"/>
+      <c r="DO21" s="37"/>
+      <c r="DP21" s="38"/>
+      <c r="DQ21" s="40"/>
+      <c r="DR21" s="40"/>
+      <c r="DS21" s="40"/>
+      <c r="DT21" s="40"/>
+    </row>
+    <row r="22" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="40"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="40"/>
+      <c r="AB22" s="38"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="40"/>
+      <c r="AQ22" s="39"/>
+      <c r="AR22" s="39"/>
+      <c r="AS22" s="35"/>
+      <c r="AT22" s="39"/>
+      <c r="AU22" s="40"/>
+      <c r="BF22" s="39"/>
+      <c r="BG22" s="39"/>
+      <c r="BH22" s="39"/>
+      <c r="BI22" s="39"/>
+      <c r="BJ22" s="40"/>
+      <c r="BU22" s="39"/>
+      <c r="BV22" s="39"/>
+      <c r="BW22" s="35"/>
+      <c r="BX22" s="39"/>
+      <c r="BY22" s="40"/>
+      <c r="CM22" s="37"/>
+      <c r="CN22" s="38"/>
+      <c r="CO22" s="38"/>
+      <c r="CU22" s="37"/>
+      <c r="CV22" s="38"/>
+      <c r="CW22" s="38"/>
+      <c r="DG22" s="37"/>
+      <c r="DH22" s="38"/>
+      <c r="DI22" s="38"/>
+      <c r="DO22" s="37"/>
+      <c r="DP22" s="38"/>
+      <c r="DQ22" s="38"/>
+    </row>
+    <row r="23" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="40"/>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="40"/>
+      <c r="AE23" s="40"/>
+      <c r="AF23" s="40"/>
+      <c r="AG23" s="40"/>
+      <c r="AH23" s="40"/>
+      <c r="AI23" s="40"/>
+      <c r="AJ23" s="40"/>
+      <c r="AK23" s="40"/>
+      <c r="AQ23" s="39"/>
+      <c r="AR23" s="39"/>
+      <c r="AS23" s="39"/>
+      <c r="AT23" s="40"/>
+      <c r="AU23" s="40"/>
+      <c r="AV23" s="40"/>
+      <c r="AW23" s="40"/>
+      <c r="AX23" s="40"/>
+      <c r="AY23" s="40"/>
+      <c r="AZ23" s="40"/>
+      <c r="BF23" s="39"/>
+      <c r="BG23" s="39"/>
+      <c r="BH23" s="39"/>
+      <c r="BI23" s="40"/>
+      <c r="BJ23" s="40"/>
+      <c r="BK23" s="40"/>
+      <c r="BL23" s="40"/>
+      <c r="BM23" s="40"/>
+      <c r="BN23" s="40"/>
+      <c r="BO23" s="40"/>
+      <c r="BU23" s="39"/>
+      <c r="BV23" s="39"/>
+      <c r="BW23" s="39"/>
+      <c r="BX23" s="39"/>
+      <c r="BY23" s="40"/>
+      <c r="BZ23" s="40"/>
+      <c r="CA23" s="40"/>
+      <c r="CB23" s="40"/>
+      <c r="CC23" s="40"/>
+      <c r="CD23" s="40"/>
+      <c r="CN23" s="40"/>
+      <c r="CV23" s="40"/>
+      <c r="DH23" s="40"/>
+      <c r="DP23" s="40"/>
+    </row>
+    <row r="24" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="40"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="40"/>
+      <c r="AB24" s="38"/>
+      <c r="AC24" s="38"/>
+      <c r="AD24" s="38"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="40"/>
+      <c r="AQ24" s="39"/>
+      <c r="AR24" s="39"/>
+      <c r="AS24" s="40"/>
+      <c r="AT24" s="39"/>
+      <c r="AU24" s="40"/>
+      <c r="BF24" s="39"/>
+      <c r="BG24" s="39"/>
+      <c r="BH24" s="39"/>
+      <c r="BI24" s="39"/>
+      <c r="BJ24" s="40"/>
+      <c r="BU24" s="39"/>
+      <c r="BV24" s="39"/>
+      <c r="BW24" s="40"/>
+      <c r="BX24" s="39"/>
+      <c r="BY24" s="40"/>
+      <c r="CN24" s="40"/>
+      <c r="CV24" s="40"/>
+      <c r="DH24" s="40"/>
+      <c r="DP24" s="40"/>
+    </row>
+    <row r="25" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="AB25" s="38"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="40"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AQ25" s="39"/>
+      <c r="AR25" s="40"/>
+      <c r="AS25" s="40"/>
+      <c r="AT25" s="40"/>
+      <c r="AU25" s="39"/>
+      <c r="BF25" s="39"/>
+      <c r="BG25" s="40"/>
+      <c r="BH25" s="40"/>
+      <c r="BI25" s="40"/>
+      <c r="BJ25" s="39"/>
+      <c r="BU25" s="39"/>
+      <c r="BV25" s="40"/>
+      <c r="BW25" s="40"/>
+      <c r="BX25" s="40"/>
+      <c r="BY25" s="39"/>
+      <c r="CN25" s="40"/>
+      <c r="CV25" s="40"/>
+      <c r="DH25" s="40"/>
+      <c r="DP25" s="40"/>
+    </row>
+    <row r="26" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="AD26" s="40"/>
+      <c r="AS26" s="40"/>
+      <c r="BH26" s="40"/>
+      <c r="BW26" s="40"/>
+      <c r="CN26" s="40"/>
+      <c r="CV26" s="40"/>
+      <c r="DH26" s="40"/>
+      <c r="DP26" s="40"/>
+    </row>
+    <row r="27" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="AD27" s="40"/>
+      <c r="AS27" s="40"/>
+      <c r="BH27" s="40"/>
+      <c r="BW27" s="40"/>
+    </row>
+    <row r="28" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="AD28" s="40"/>
+      <c r="AS28" s="40"/>
+      <c r="BH28" s="40"/>
+      <c r="BW28" s="40"/>
+    </row>
+    <row r="29" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="AD29" s="40"/>
+      <c r="AS29" s="40"/>
+      <c r="BH29" s="40"/>
+      <c r="BW29" s="40"/>
+    </row>
+    <row r="30" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="AD30" s="40"/>
+      <c r="AS30" s="40"/>
+      <c r="BH30" s="40"/>
+      <c r="BW30" s="40"/>
+    </row>
+    <row r="31" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="AD31" s="40"/>
+      <c r="AS31" s="40"/>
+      <c r="BH31" s="40"/>
+      <c r="BW31" s="40"/>
+      <c r="CN31" s="35"/>
+      <c r="CV31" s="35"/>
+      <c r="DH31" s="35"/>
+      <c r="DP31" s="35"/>
+    </row>
+    <row r="32" spans="3:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="AD32" s="40"/>
+      <c r="AS32" s="40"/>
+      <c r="BH32" s="40"/>
+      <c r="BW32" s="40"/>
+      <c r="CN32" s="35"/>
+      <c r="CV32" s="35"/>
+      <c r="DH32" s="35"/>
+      <c r="DP32" s="35"/>
+    </row>
+    <row r="33" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN33" s="35"/>
+      <c r="CV33" s="35"/>
+      <c r="DH33" s="35"/>
+      <c r="DP33" s="35"/>
+    </row>
+    <row r="34" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN34" s="35"/>
+      <c r="CV34" s="35"/>
+      <c r="DH34" s="35"/>
+      <c r="DP34" s="35"/>
+    </row>
+    <row r="35" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CM35" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="CN35" s="38"/>
+      <c r="CO35" s="38"/>
+      <c r="CU35" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="CV35" s="38"/>
+      <c r="CW35" s="38"/>
+      <c r="DG35" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="DH35" s="38"/>
+      <c r="DI35" s="38"/>
+      <c r="DO35" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="DP35" s="38"/>
+      <c r="DQ35" s="38"/>
+    </row>
+    <row r="36" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CM36" s="37"/>
+      <c r="CN36" s="38"/>
+      <c r="CO36" s="35"/>
+      <c r="CP36" s="35"/>
+      <c r="CQ36" s="35"/>
+      <c r="CR36" s="35"/>
+      <c r="CU36" s="37"/>
+      <c r="CV36" s="38"/>
+      <c r="CW36" s="41"/>
+      <c r="CX36" s="41"/>
+      <c r="CY36" s="41"/>
+      <c r="CZ36" s="41"/>
+      <c r="DG36" s="37"/>
+      <c r="DH36" s="38"/>
+      <c r="DI36" s="35"/>
+      <c r="DJ36" s="35"/>
+      <c r="DK36" s="35"/>
+      <c r="DL36" s="35"/>
+      <c r="DO36" s="37"/>
+      <c r="DP36" s="38"/>
+      <c r="DQ36" s="41"/>
+      <c r="DR36" s="41"/>
+      <c r="DS36" s="41"/>
+      <c r="DT36" s="41"/>
+    </row>
+    <row r="37" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CM37" s="37"/>
+      <c r="CN37" s="38"/>
+      <c r="CO37" s="38"/>
+      <c r="CU37" s="37"/>
+      <c r="CV37" s="38"/>
+      <c r="CW37" s="38"/>
+      <c r="DG37" s="37"/>
+      <c r="DH37" s="38"/>
+      <c r="DI37" s="38"/>
+      <c r="DO37" s="37"/>
+      <c r="DP37" s="38"/>
+      <c r="DQ37" s="38"/>
+    </row>
+    <row r="38" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN38" s="41"/>
+      <c r="CV38" s="41"/>
+      <c r="DH38" s="42"/>
+      <c r="DP38" s="41"/>
+    </row>
+    <row r="39" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN39" s="41"/>
+      <c r="CV39" s="41"/>
+      <c r="DH39" s="42"/>
+      <c r="DP39" s="41"/>
+    </row>
+    <row r="40" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN40" s="41"/>
+      <c r="CV40" s="41"/>
+      <c r="DH40" s="42"/>
+      <c r="DP40" s="41"/>
+    </row>
+    <row r="41" spans="91:124" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="CN41" s="41"/>
+      <c r="CV41" s="41"/>
+      <c r="DH41" s="42"/>
+      <c r="DP41" s="41"/>
+    </row>
+    <row r="55" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BM55" s="41"/>
+    </row>
+    <row r="56" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BM56" s="41"/>
+    </row>
+    <row r="57" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BM57" s="41"/>
+    </row>
+    <row r="58" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BI58" s="43"/>
+      <c r="BJ58" s="43"/>
+      <c r="BK58" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL58" s="43"/>
+      <c r="BM58" s="38"/>
+      <c r="BN58" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="CF58" s="41"/>
+    </row>
+    <row r="59" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG59" s="35"/>
+      <c r="BH59" s="35"/>
+      <c r="BI59" s="35"/>
+      <c r="BJ59" s="43"/>
+      <c r="BK59" s="44"/>
+      <c r="BL59" s="41"/>
+      <c r="BM59" s="38"/>
+      <c r="BN59" s="44"/>
+      <c r="CF59" s="41"/>
+    </row>
+    <row r="60" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG60" s="35"/>
+      <c r="BI60" s="43"/>
+      <c r="BJ60" s="43"/>
+      <c r="BK60" s="44"/>
+      <c r="BL60" s="43"/>
+      <c r="BM60" s="38"/>
+      <c r="BN60" s="44"/>
+      <c r="CF60" s="41"/>
+    </row>
+    <row r="61" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG61" s="35"/>
+      <c r="BM61" s="41"/>
+      <c r="CB61" s="43"/>
+      <c r="CC61" s="43"/>
+      <c r="CD61" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE61" s="43"/>
+      <c r="CF61" s="38"/>
+      <c r="CG61" s="44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG62" s="35"/>
+      <c r="BM62" s="41"/>
+      <c r="BN62" s="41"/>
+      <c r="BO62" s="41"/>
+      <c r="BP62" s="41"/>
+      <c r="BQ62" s="41"/>
+      <c r="BZ62" s="35"/>
+      <c r="CA62" s="35"/>
+      <c r="CB62" s="35"/>
+      <c r="CC62" s="43"/>
+      <c r="CD62" s="44"/>
+      <c r="CE62" s="41"/>
+      <c r="CF62" s="38"/>
+      <c r="CG62" s="44"/>
+    </row>
+    <row r="63" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG63" s="35"/>
+      <c r="BM63" s="41"/>
+      <c r="BZ63" s="35"/>
+      <c r="CB63" s="43"/>
+      <c r="CC63" s="43"/>
+      <c r="CD63" s="44"/>
+      <c r="CE63" s="43"/>
+      <c r="CF63" s="38"/>
+      <c r="CG63" s="44"/>
+    </row>
+    <row r="64" spans="58:85" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BF64" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG64" s="38"/>
+      <c r="BH64" s="38"/>
+      <c r="BI64" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="BJ64" s="38"/>
+      <c r="BK64" s="38"/>
+      <c r="BM64" s="41"/>
+      <c r="BY64" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ64" s="38"/>
+      <c r="CA64" s="38"/>
+      <c r="CB64" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC64" s="38"/>
+      <c r="CD64" s="38"/>
+      <c r="CF64" s="41"/>
+    </row>
+    <row r="65" spans="58:88" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BF65" s="37"/>
+      <c r="BG65" s="38"/>
+      <c r="BH65" s="35"/>
+      <c r="BI65" s="37"/>
+      <c r="BJ65" s="38"/>
+      <c r="BK65" s="41"/>
+      <c r="BL65" s="41"/>
+      <c r="BM65" s="41"/>
+      <c r="BY65" s="37"/>
+      <c r="BZ65" s="38"/>
+      <c r="CA65" s="35"/>
+      <c r="CB65" s="37"/>
+      <c r="CC65" s="38"/>
+      <c r="CD65" s="41"/>
+      <c r="CE65" s="41"/>
+      <c r="CF65" s="41"/>
+      <c r="CG65" s="41"/>
+      <c r="CH65" s="41"/>
+      <c r="CI65" s="41"/>
+      <c r="CJ65" s="41"/>
+    </row>
+    <row r="66" spans="58:88" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BF66" s="37"/>
+      <c r="BG66" s="38"/>
+      <c r="BH66" s="38"/>
+      <c r="BI66" s="37"/>
+      <c r="BJ66" s="38"/>
+      <c r="BK66" s="38"/>
+      <c r="BY66" s="37"/>
+      <c r="BZ66" s="38"/>
+      <c r="CA66" s="38"/>
+      <c r="CB66" s="37"/>
+      <c r="CC66" s="38"/>
+      <c r="CD66" s="38"/>
+    </row>
+    <row r="67" spans="58:88" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG67" s="35"/>
+      <c r="BZ67" s="35"/>
+    </row>
+    <row r="68" spans="58:88" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG68" s="35"/>
+      <c r="BZ68" s="35"/>
+    </row>
+    <row r="69" spans="58:88" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BG69" s="35"/>
+      <c r="BZ69" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="CG61:CG63"/>
+    <mergeCell ref="BY64:BY66"/>
+    <mergeCell ref="CB64:CB66"/>
+    <mergeCell ref="BF64:BF66"/>
+    <mergeCell ref="BI64:BI66"/>
+    <mergeCell ref="BN58:BN60"/>
+    <mergeCell ref="BK58:BK60"/>
+    <mergeCell ref="CD61:CD63"/>
+    <mergeCell ref="CM20:CM22"/>
+    <mergeCell ref="CU20:CU22"/>
+    <mergeCell ref="DG20:DG22"/>
+    <mergeCell ref="DO20:DO22"/>
+    <mergeCell ref="CM35:CM37"/>
+    <mergeCell ref="CU35:CU37"/>
+    <mergeCell ref="DG35:DG37"/>
+    <mergeCell ref="DO35:DO37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>